<commit_message>
Improve data import process to function in different execution contexts
Modify import_snap_lotto_data.py to handle database operations conditionally based on Flask app context to avoid errors in standalone mode.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7242c9e3-1c7d-4770-bc2a-a542c4aeed2f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/45399ea3-630c-4463-8e3d-edea73bb30a7/472c2617-6cef-4eba-bee6-24c654615107.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/lottery_test_data.xlsx
+++ b/attached_assets/lottery_test_data.xlsx
@@ -514,54 +514,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1649</t>
+          <t>1322</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2, 48, 5, 29, 2, 7</t>
+          <t>20, 33, 22, 23, 3, 48</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R24,712,158.00</t>
+          <t>R29,226,741.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R449,379.00</t>
+          <t>R67,212.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R8,834.00</t>
+          <t>R5,618.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R82,298,151.00</t>
+          <t>R66,164,895.00</t>
         </is>
       </c>
     </row>
@@ -573,54 +573,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1650</t>
+          <t>1323</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5, 16, 25, 7, 21, 37</t>
+          <t>26, 13, 33, 25, 48, 21</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R40,599,353.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R310,447.00</t>
+          <t>R417,512.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>326</v>
+        <v>472</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R9,114.00</t>
+          <t>R5,883.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R14,805,378.00</t>
+          <t>R20,681,283.00</t>
         </is>
       </c>
     </row>
@@ -632,54 +632,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>1324</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>27, 41, 41, 41, 10, 14</t>
+          <t>39, 27, 2, 27, 52, 50</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R3,534,802.00</t>
+          <t>R40,098,575.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R99,549.00</t>
+          <t>R388,087.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>424</v>
+        <v>281</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R2,589.00</t>
+          <t>R6,731.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R73,055,506.00</t>
+          <t>R18,013,697.00</t>
         </is>
       </c>
     </row>
@@ -691,54 +691,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1652</t>
+          <t>1325</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>50, 23, 51, 36, 23, 7</t>
+          <t>12, 10, 25, 4, 20, 1</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R16,747,079.00</t>
+          <t>R41,854,556.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R97,376.00</t>
+          <t>R435,932.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>333</v>
+        <v>166</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R6,954.00</t>
+          <t>R5,224.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R69,935,281.00</t>
+          <t>R81,456,424.00</t>
         </is>
       </c>
     </row>
@@ -750,54 +750,54 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1653</t>
+          <t>1326</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>30, 10, 5, 34, 32, 5</t>
+          <t>14, 34, 50, 52, 46, 16</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R49,149,912.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R495,189.00</t>
+          <t>R314,960.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R7,442.00</t>
+          <t>R3,193.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R81,690,939.00</t>
+          <t>R87,878,087.00</t>
         </is>
       </c>
     </row>
@@ -895,54 +895,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1503</t>
+          <t>1055</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>30, 18, 18, 33, 40, 18</t>
+          <t>5, 21, 2, 48, 6, 42</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R18,205,496.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R499,124.00</t>
+          <t>R75,298.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>143</v>
+        <v>435</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R3,544.00</t>
+          <t>R2,424.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R14,996,836.00</t>
+          <t>R79,813,056.00</t>
         </is>
       </c>
     </row>
@@ -954,54 +954,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1504</t>
+          <t>1056</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>23, 14, 47, 9, 38, 6</t>
+          <t>48, 12, 8, 43, 45, 42</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R45,000,828.00</t>
+          <t>R29,109,166.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R166,965.00</t>
+          <t>R178,249.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>331</v>
+        <v>180</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R2,902.00</t>
+          <t>R9,256.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R46,585,877.00</t>
+          <t>R22,162,309.00</t>
         </is>
       </c>
     </row>
@@ -1013,21 +1013,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1505</t>
+          <t>1057</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1, 45, 42, 35, 20, 14</t>
+          <t>27, 36, 34, 19, 41, 17</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1038,29 +1038,29 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R156,065.00</t>
+          <t>R300,175.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>253</v>
+        <v>475</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R2,297.00</t>
+          <t>R8,754.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R44,016,678.00</t>
+          <t>R25,103,372.00</t>
         </is>
       </c>
     </row>
@@ -1072,21 +1072,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1506</t>
+          <t>1058</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>45, 16, 20, 24, 32, 16</t>
+          <t>44, 11, 4, 21, 38, 37</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1097,29 +1097,29 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R238,896.00</t>
+          <t>R299,010.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>441</v>
+        <v>194</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R5,233.00</t>
+          <t>R4,528.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R20,608,971.00</t>
+          <t>R41,870,931.00</t>
         </is>
       </c>
     </row>
@@ -1131,54 +1131,54 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1507</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3, 37, 15, 6, 8, 8</t>
+          <t>46, 38, 14, 45, 30, 12</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R47,429,489.00</t>
+          <t>R12,534,996.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R473,300.00</t>
+          <t>R250,005.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>111</v>
+        <v>359</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R2,270.00</t>
+          <t>R4,929.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R53,305,745.00</t>
+          <t>R54,478,368.00</t>
         </is>
       </c>
     </row>
@@ -1276,54 +1276,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1748</t>
+          <t>1824</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>44, 49, 10, 2, 9, 30</t>
+          <t>44, 30, 33, 42, 41, 27</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R25,099,500.00</t>
+          <t>R22,554,398.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R260,937.00</t>
+          <t>R250,348.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>358</v>
+        <v>211</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R5,183.00</t>
+          <t>R3,726.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R53,692,339.00</t>
+          <t>R88,989,872.00</t>
         </is>
       </c>
     </row>
@@ -1335,54 +1335,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1749</t>
+          <t>1825</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6, 40, 5, 7, 21, 34</t>
+          <t>33, 42, 40, 38, 50, 5</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R46,689,189.00</t>
+          <t>R39,139,880.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R479,108.00</t>
+          <t>R336,965.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>476</v>
+        <v>110</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R6,090.00</t>
+          <t>R8,183.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R72,344,175.00</t>
+          <t>R47,766,681.00</t>
         </is>
       </c>
     </row>
@@ -1394,54 +1394,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1750</t>
+          <t>1826</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>32, 50, 49, 43, 46, 19</t>
+          <t>23, 16, 29, 44, 10, 51</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R22,826,730.00</t>
+          <t>R30,694,647.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R190,590.00</t>
+          <t>R432,655.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R6,862.00</t>
+          <t>R4,763.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R15,675,536.00</t>
+          <t>R84,552,076.00</t>
         </is>
       </c>
     </row>
@@ -1453,54 +1453,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1751</t>
+          <t>1827</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>45, 27, 52, 9, 20, 36</t>
+          <t>48, 3, 33, 11, 22, 36</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R3,341,480.00</t>
+          <t>R12,885,252.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R336,028.00</t>
+          <t>R289,700.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>317</v>
+        <v>188</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R1,470.00</t>
+          <t>R8,613.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R60,288,317.00</t>
+          <t>R41,791,155.00</t>
         </is>
       </c>
     </row>
@@ -1512,21 +1512,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1752</t>
+          <t>1828</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>18, 26, 35, 11, 27, 17</t>
+          <t>16, 45, 40, 5, 28, 49</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1537,29 +1537,29 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R334,506.00</t>
+          <t>R192,090.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>468</v>
+        <v>312</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R2,566.00</t>
+          <t>R8,780.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R75,922,713.00</t>
+          <t>R82,401,159.00</t>
         </is>
       </c>
     </row>
@@ -1657,54 +1657,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1712</t>
+          <t>1729</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>21, 18, 26, 14, 31</t>
+          <t>21, 14, 45, 30, 47</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R30,828,795.00</t>
+          <t>R43,107,133.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R94,703.00</t>
+          <t>R455,967.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>115</v>
+        <v>418</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R7,608.00</t>
+          <t>R8,440.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R66,427,341.00</t>
+          <t>R19,105,477.00</t>
         </is>
       </c>
     </row>
@@ -1716,54 +1716,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1713</t>
+          <t>1730</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3, 6, 37, 40, 23</t>
+          <t>22, 48, 38, 37, 45</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R6,079,640.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R123,801.00</t>
+          <t>R168,453.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R2,245.00</t>
+          <t>R2,153.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R70,463,063.00</t>
+          <t>R35,208,894.00</t>
         </is>
       </c>
     </row>
@@ -1775,54 +1775,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>1731</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14, 2, 46, 43, 9</t>
+          <t>23, 42, 43, 10, 5</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R22,142,989.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R416,715.00</t>
+          <t>R65,187.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R7,140.00</t>
+          <t>R1,462.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R63,796,107.00</t>
+          <t>R89,526,787.00</t>
         </is>
       </c>
     </row>
@@ -1834,21 +1834,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1715</t>
+          <t>1732</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2, 15, 19, 49, 25</t>
+          <t>46, 24, 8, 38, 47</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1859,29 +1859,29 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R346,891.00</t>
+          <t>R381,281.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>455</v>
+        <v>147</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R2,838.00</t>
+          <t>R4,488.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R12,781,102.00</t>
+          <t>R82,239,779.00</t>
         </is>
       </c>
     </row>
@@ -1893,54 +1893,54 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1716</t>
+          <t>1733</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3, 36, 20, 14, 41</t>
+          <t>14, 7, 37, 26, 35</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R21,782,649.00</t>
+          <t>R11,115,404.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R449,457.00</t>
+          <t>R403,384.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R6,128.00</t>
+          <t>R5,754.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R26,909,796.00</t>
+          <t>R36,048,809.00</t>
         </is>
       </c>
     </row>
@@ -2038,54 +2038,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1307</t>
+          <t>1354</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>43, 24, 22, 20, 29</t>
+          <t>49, 44, 20, 4, 50</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R22,592,726.00</t>
+          <t>R25,059,687.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R487,902.00</t>
+          <t>R153,375.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>135</v>
+        <v>319</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R9,450.00</t>
+          <t>R9,961.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R68,729,422.00</t>
+          <t>R55,139,751.00</t>
         </is>
       </c>
     </row>
@@ -2097,54 +2097,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>1355</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-04</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>33, 23, 32, 28, 3</t>
+          <t>43, 34, 3, 5, 1</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R45,159,334.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R420,297.00</t>
+          <t>R419,361.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>257</v>
+        <v>424</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R3,146.00</t>
+          <t>R4,853.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R80,767,051.00</t>
+          <t>R39,152,764.00</t>
         </is>
       </c>
     </row>
@@ -2156,54 +2156,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1356</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>43, 49, 19, 14, 48</t>
+          <t>7, 42, 22, 44, 50</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R45,080,179.00</t>
+          <t>R10,918,093.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R280,228.00</t>
+          <t>R292,780.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>212</v>
+        <v>339</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R9,604.00</t>
+          <t>R6,650.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R61,395,335.00</t>
+          <t>R62,414,729.00</t>
         </is>
       </c>
     </row>
@@ -2215,54 +2215,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1310</t>
+          <t>1357</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>42, 26, 22, 32, 7</t>
+          <t>36, 50, 11, 44, 50</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R45,119,265.00</t>
+          <t>R17,557,382.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R361,767.00</t>
+          <t>R182,598.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>482</v>
+        <v>112</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R5,746.00</t>
+          <t>R9,481.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R12,510,679.00</t>
+          <t>R94,922,920.00</t>
         </is>
       </c>
     </row>
@@ -2274,54 +2274,54 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1311</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>46, 19, 7, 8, 36</t>
+          <t>13, 40, 20, 35, 35</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R7,965,102.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R113,099.00</t>
+          <t>R199,593.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R1,629.00</t>
+          <t>R6,162.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R61,277,224.00</t>
+          <t>R25,562,326.00</t>
         </is>
       </c>
     </row>
@@ -2419,52 +2419,52 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1370</t>
+          <t>1481</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10, 17, 34, 5, 28</t>
+          <t>25, 8, 2, 10, 18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R30,609,700.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R483,004.00</t>
+          <t>R448,150.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>415</v>
+        <v>288</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R8,664.00</t>
+          <t>R4,734.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-02-26</t>
+          <t>2025-02-27</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R35,684,397.00</t>
+          <t>R89,378,863.00</t>
         </is>
       </c>
     </row>
@@ -2476,52 +2476,52 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1371</t>
+          <t>1482</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-02-26</t>
+          <t>2025-02-27</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>34, 5, 7, 34, 35</t>
+          <t>21, 26, 36, 4, 31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R40,291,705.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R90,308.00</t>
+          <t>R289,531.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R9,695.00</t>
+          <t>R3,610.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-02-27</t>
+          <t>2025-02-28</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R16,369,133.00</t>
+          <t>R69,737,228.00</t>
         </is>
       </c>
     </row>
@@ -2533,52 +2533,52 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1372</t>
+          <t>1483</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-02-27</t>
+          <t>2025-02-28</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13, 16, 9, 24, 10</t>
+          <t>3, 19, 20, 32, 10</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R37,716,985.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R338,673.00</t>
+          <t>R300,072.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>238</v>
+        <v>341</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R1,521.00</t>
+          <t>R5,324.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-02-28</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R38,096,797.00</t>
+          <t>R95,015,163.00</t>
         </is>
       </c>
     </row>
@@ -2590,52 +2590,52 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1373</t>
+          <t>1484</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-02-28</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24, 27, 32, 27, 4</t>
+          <t>16, 24, 18, 35, 10</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R14,595,832.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R96,168.00</t>
+          <t>R93,099.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>192</v>
+        <v>291</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R5,514.00</t>
+          <t>R7,675.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2025-03-02</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R68,357,597.00</t>
+          <t>R74,976,933.00</t>
         </is>
       </c>
     </row>
@@ -2647,52 +2647,52 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1374</t>
+          <t>1485</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2025-03-02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2, 12, 6, 26, 34</t>
+          <t>35, 35, 3, 32, 26</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R26,762,735.00</t>
+          <t>R38,407,089.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R291,944.00</t>
+          <t>R229,196.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R7,451.00</t>
+          <t>R2,524.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-03-03</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R78,042,672.00</t>
+          <t>R60,234,420.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ensure initial data and assets are included within the deployment package
Add initial data, test datasets, database, analysis images and upload assets.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7242c9e3-1c7d-4770-bc2a-a542c4aeed2f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/45399ea3-630c-4463-8e3d-edea73bb30a7/6b0ba02f-bda4-49d8-b86e-622a213bcddd.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/lottery_test_data.xlsx
+++ b/attached_assets/lottery_test_data.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1322</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -524,34 +524,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20, 33, 22, 23, 3, 48</t>
+          <t>34, 25, 17, 27, 25, 26</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R29,226,741.00</t>
+          <t>R18,996,600.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R67,212.00</t>
+          <t>R159,980.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>308</v>
+        <v>158</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R5,618.00</t>
+          <t>R3,697.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R66,164,895.00</t>
+          <t>R29,716,257.00</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1323</t>
+          <t>1331</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -583,11 +583,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>26, 13, 33, 25, 48, 21</t>
+          <t>20, 22, 10, 33, 11, 14</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -598,19 +598,19 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R417,512.00</t>
+          <t>R465,466.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>472</v>
+        <v>109</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R5,883.00</t>
+          <t>R9,728.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R20,681,283.00</t>
+          <t>R4,440,409.00</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>1332</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -642,34 +642,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>39, 27, 2, 27, 52, 50</t>
+          <t>38, 1, 32, 17, 10, 42</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R40,098,575.00</t>
+          <t>R15,058,478.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R388,087.00</t>
+          <t>R375,557.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>281</v>
+        <v>230</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R6,731.00</t>
+          <t>R7,402.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R18,013,697.00</t>
+          <t>R22,143,756.00</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1325</t>
+          <t>1333</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -701,34 +701,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12, 10, 25, 4, 20, 1</t>
+          <t>9, 21, 47, 28, 10, 50</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R41,854,556.00</t>
+          <t>R27,517,558.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R435,932.00</t>
+          <t>R432,670.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R5,224.00</t>
+          <t>R6,842.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R81,456,424.00</t>
+          <t>R91,131,012.00</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1326</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -760,34 +760,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14, 34, 50, 52, 46, 16</t>
+          <t>31, 51, 4, 44, 38, 50</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R49,149,912.00</t>
+          <t>R35,288,200.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R314,960.00</t>
+          <t>R264,859.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>157</v>
+        <v>400</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R3,193.00</t>
+          <t>R2,013.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R87,878,087.00</t>
+          <t>R17,652,716.00</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1055</t>
+          <t>1706</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -905,34 +905,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5, 21, 2, 48, 6, 42</t>
+          <t>43, 44, 33, 9, 2, 46</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R44,911,903.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R75,298.00</t>
+          <t>R472,105.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>435</v>
+        <v>367</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R2,424.00</t>
+          <t>R6,684.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R79,813,056.00</t>
+          <t>R24,580,845.00</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1056</t>
+          <t>1707</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -964,34 +964,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>48, 12, 8, 43, 45, 42</t>
+          <t>39, 14, 16, 42, 5, 30</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R29,109,166.00</t>
+          <t>R22,381,310.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R178,249.00</t>
+          <t>R169,164.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>180</v>
+        <v>325</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R9,256.00</t>
+          <t>R4,383.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R22,162,309.00</t>
+          <t>R93,934,238.00</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1057</t>
+          <t>1708</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1023,34 +1023,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>27, 36, 34, 19, 41, 17</t>
+          <t>17, 19, 28, 18, 18, 14</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R28,356,316.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R300,175.00</t>
+          <t>R156,612.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>475</v>
+        <v>419</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R8,754.00</t>
+          <t>R4,427.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R25,103,372.00</t>
+          <t>R32,439,450.00</t>
         </is>
       </c>
     </row>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1058</t>
+          <t>1709</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1082,34 +1082,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>44, 11, 4, 21, 38, 37</t>
+          <t>51, 13, 1, 7, 23, 25</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R21,498,313.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R299,010.00</t>
+          <t>R273,394.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>194</v>
+        <v>394</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R4,528.00</t>
+          <t>R4,354.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R41,870,931.00</t>
+          <t>R45,030,954.00</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1059</t>
+          <t>1710</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1141,34 +1141,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>46, 38, 14, 45, 30, 12</t>
+          <t>10, 21, 52, 31, 52, 49</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R12,534,996.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R250,005.00</t>
+          <t>R372,258.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>359</v>
+        <v>430</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R4,929.00</t>
+          <t>R1,257.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R54,478,368.00</t>
+          <t>R38,981,106.00</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1824</t>
+          <t>1270</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1286,34 +1286,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>44, 30, 33, 42, 41, 27</t>
+          <t>52, 2, 39, 50, 6, 42</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R22,554,398.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R250,348.00</t>
+          <t>R313,645.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>211</v>
+        <v>434</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R3,726.00</t>
+          <t>R9,981.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R88,989,872.00</t>
+          <t>R39,422,277.00</t>
         </is>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1825</t>
+          <t>1271</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1345,34 +1345,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>33, 42, 40, 38, 50, 5</t>
+          <t>34, 15, 40, 4, 34, 12</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R39,139,880.00</t>
+          <t>R22,584,471.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R336,965.00</t>
+          <t>R303,070.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>110</v>
+        <v>362</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R8,183.00</t>
+          <t>R9,523.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R47,766,681.00</t>
+          <t>R17,608,069.00</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>1272</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1404,34 +1404,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>23, 16, 29, 44, 10, 51</t>
+          <t>11, 42, 24, 30, 20, 43</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R30,694,647.00</t>
+          <t>R23,264,118.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R432,655.00</t>
+          <t>R289,224.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>175</v>
+        <v>451</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R4,763.00</t>
+          <t>R6,185.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R84,552,076.00</t>
+          <t>R67,414,780.00</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1827</t>
+          <t>1273</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1463,34 +1463,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>48, 3, 33, 11, 22, 36</t>
+          <t>47, 49, 52, 2, 52, 4</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R12,885,252.00</t>
+          <t>R5,641,485.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R289,700.00</t>
+          <t>R430,599.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>188</v>
+        <v>268</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R8,613.00</t>
+          <t>R2,840.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R41,791,155.00</t>
+          <t>R47,739,447.00</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1828</t>
+          <t>1274</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1522,34 +1522,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>16, 45, 40, 5, 28, 49</t>
+          <t>45, 34, 36, 48, 30, 45</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R44,061,661.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R192,090.00</t>
+          <t>R409,467.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>312</v>
+        <v>359</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R8,780.00</t>
+          <t>R2,363.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R82,401,159.00</t>
+          <t>R92,753,862.00</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1729</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1667,34 +1667,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>21, 14, 45, 30, 47</t>
+          <t>28, 43, 49, 41, 9</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R43,107,133.00</t>
+          <t>R33,246,160.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R455,967.00</t>
+          <t>R414,130.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>418</v>
+        <v>293</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R8,440.00</t>
+          <t>R9,433.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R19,105,477.00</t>
+          <t>R67,762,649.00</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1730</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1726,34 +1726,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>22, 48, 38, 37, 45</t>
+          <t>19, 2, 29, 40, 27</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R13,196,501.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R168,453.00</t>
+          <t>R437,169.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>398</v>
+        <v>197</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R2,153.00</t>
+          <t>R6,942.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R35,208,894.00</t>
+          <t>R57,776,677.00</t>
         </is>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1731</t>
+          <t>1722</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1785,34 +1785,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>23, 42, 43, 10, 5</t>
+          <t>13, 3, 7, 50, 17</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R17,141,277.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R65,187.00</t>
+          <t>R50,055.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R1,462.00</t>
+          <t>R5,608.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R89,526,787.00</t>
+          <t>R75,294,491.00</t>
         </is>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1732</t>
+          <t>1723</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1844,34 +1844,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>46, 24, 8, 38, 47</t>
+          <t>46, 12, 25, 19, 24</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R11,006,294.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R381,281.00</t>
+          <t>R61,284.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>147</v>
+        <v>415</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R4,488.00</t>
+          <t>R2,566.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R82,239,779.00</t>
+          <t>R40,679,950.00</t>
         </is>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1733</t>
+          <t>1724</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1903,34 +1903,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14, 7, 37, 26, 35</t>
+          <t>32, 49, 50, 1, 7</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R11,115,404.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R403,384.00</t>
+          <t>R311,617.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>266</v>
+        <v>442</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R5,754.00</t>
+          <t>R7,480.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R36,048,809.00</t>
+          <t>R96,698,661.00</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1354</t>
+          <t>1648</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2048,34 +2048,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>49, 44, 20, 4, 50</t>
+          <t>23, 46, 44, 19, 30</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R25,059,687.00</t>
+          <t>R45,070,912.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R153,375.00</t>
+          <t>R286,426.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>319</v>
+        <v>273</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R9,961.00</t>
+          <t>R5,159.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R55,139,751.00</t>
+          <t>R77,337,892.00</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1355</t>
+          <t>1649</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2107,11 +2107,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>43, 34, 3, 5, 1</t>
+          <t>36, 37, 46, 34, 20</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -2122,19 +2122,19 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R419,361.00</t>
+          <t>R99,909.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>424</v>
+        <v>351</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R4,853.00</t>
+          <t>R4,340.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R39,152,764.00</t>
+          <t>R16,968,525.00</t>
         </is>
       </c>
     </row>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1356</t>
+          <t>1650</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2166,34 +2166,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>7, 42, 22, 44, 50</t>
+          <t>1, 42, 8, 40, 49</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R10,918,093.00</t>
+          <t>R40,479,159.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R292,780.00</t>
+          <t>R132,153.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>339</v>
+        <v>396</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R6,650.00</t>
+          <t>R1,742.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R62,414,729.00</t>
+          <t>R74,181,750.00</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1357</t>
+          <t>1651</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2225,34 +2225,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>36, 50, 11, 44, 50</t>
+          <t>15, 45, 23, 3, 20</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R17,557,382.00</t>
+          <t>R5,735,780.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R182,598.00</t>
+          <t>R161,398.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R9,481.00</t>
+          <t>R8,193.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R94,922,920.00</t>
+          <t>R93,310,679.00</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>1652</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2284,34 +2284,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13, 40, 20, 35, 35</t>
+          <t>17, 44, 7, 22, 48</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R7,965,102.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R199,593.00</t>
+          <t>R124,800.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>394</v>
+        <v>306</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R6,162.00</t>
+          <t>R3,506.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R25,562,326.00</t>
+          <t>R19,320,040.00</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1481</t>
+          <t>1903</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2429,32 +2429,32 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>25, 8, 2, 10, 18</t>
+          <t>6, 22, 32, 27, 4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R6,175,738.00</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>R448,150.00</t>
+          <t>R340,224.00</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R4,734.00</t>
+          <t>R6,464.00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>R89,378,863.00</t>
+          <t>R93,289,648.00</t>
         </is>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1482</t>
+          <t>1904</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2486,32 +2486,32 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21, 26, 36, 4, 31</t>
+          <t>8, 25, 36, 22, 28</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R40,291,705.00</t>
+          <t>R20,843,815.00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>R289,531.00</t>
+          <t>R402,679.00</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R3,610.00</t>
+          <t>R2,650.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>R69,737,228.00</t>
+          <t>R76,583,225.00</t>
         </is>
       </c>
     </row>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1483</t>
+          <t>1905</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2543,32 +2543,32 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3, 19, 20, 32, 10</t>
+          <t>28, 17, 32, 8, 6</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R0.00</t>
+          <t>R6,841,339.00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>R300,072.00</t>
+          <t>R100,897.00</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>341</v>
+        <v>402</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R5,324.00</t>
+          <t>R7,464.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>R95,015,163.00</t>
+          <t>R21,165,034.00</t>
         </is>
       </c>
     </row>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1484</t>
+          <t>1906</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2600,32 +2600,32 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>16, 24, 18, 35, 10</t>
+          <t>11, 12, 26, 19, 10</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R14,595,832.00</t>
+          <t>R0.00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>R93,099.00</t>
+          <t>R491,846.00</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>291</v>
+        <v>369</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R7,675.00</t>
+          <t>R5,195.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>R74,976,933.00</t>
+          <t>R62,181,890.00</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1485</t>
+          <t>1907</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2657,32 +2657,32 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>35, 35, 3, 32, 26</t>
+          <t>12, 8, 30, 17, 13</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R38,407,089.00</t>
+          <t>R45,490,916.00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>R229,196.00</t>
+          <t>R197,472.00</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>201</v>
+        <v>106</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R2,524.00</t>
+          <t>R4,923.00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>R60,234,420.00</t>
+          <t>R22,395,642.00</t>
         </is>
       </c>
     </row>

</xml_diff>